<commit_message>
fix(Examples): Update default and coral reef light campaign configs and storage
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -617,7 +617,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="194">
   <si>
-    <t xml:space="preserve">SoundScapeExplorer
+    <t xml:space="preserve">CoralSoundExplorer
 Version 12</t>
   </si>
   <si>
@@ -637,7 +637,7 @@
     <t xml:space="preserve">Documentation</t>
   </si>
   <si>
-    <t xml:space="preserve">https://sound-scape-explorer.github.io/</t>
+    <t xml:space="preserve">https://sound-scape-explorer.github.io/docs/CSE/</t>
   </si>
   <si>
     <t xml:space="preserve">Campaign user guide</t>
@@ -1858,7 +1858,7 @@
     <mergeCell ref="A7:A9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="https://sound-scape-explorer.github.io/"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://sound-scape-explorer.github.io/docs/CSE/"/>
     <hyperlink ref="B13" r:id="rId2" display="https://sound-scape-explorer.github.io/docs/modules/campaign/user-guide/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix(Examples/CoralReefLight): Remove unused extractors and digesters + Regenerate h5
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -615,10 +615,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="164">
   <si>
     <t xml:space="preserve">CoralSoundExplorer
-Version 12</t>
+Version 1</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>
@@ -1180,100 +1180,10 @@
     <t xml:space="preserve">hdbscan-leaf</t>
   </si>
   <si>
-    <t xml:space="preserve">indicator</t>
-  </si>
-  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
     <t xml:space="preserve">The VGGish neural network.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leq_maad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Leq using maad library.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">med</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The temporal median.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The temporal entropy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The frequency entropy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The acoustic complexity index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The acoustic diversity index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The bioacoustics index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndsi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The normalized difference soundscape index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sum variance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sum_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The sum standard deviation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The mean standard deviation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_spreading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The mean spreading.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The distance between subtypes of a given cluster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overlap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The overlap between subtypes of a given cluster.</t>
   </si>
   <si>
     <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
@@ -2079,10 +1989,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>158</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,72 +2000,32 @@
         <v>141</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>162</v>
-      </c>
+      <c r="B3" s="48"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>164</v>
-      </c>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>166</v>
-      </c>
+      <c r="B5" s="48"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>168</v>
-      </c>
+      <c r="B6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>170</v>
-      </c>
+      <c r="B7" s="49"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>172</v>
-      </c>
+      <c r="B8" s="49"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>174</v>
-      </c>
+      <c r="B9" s="49"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="44" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>176</v>
-      </c>
+      <c r="B10" s="49"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2193,75 +2063,45 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="44" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>183</v>
-      </c>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>185</v>
-      </c>
+      <c r="B5" s="48"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>187</v>
-      </c>
+      <c r="B6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>189</v>
-      </c>
+      <c r="B7" s="48"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>190</v>
-      </c>
+      <c r="B8" s="48"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>191</v>
-      </c>
+      <c r="B9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="49"/>
@@ -2311,7 +2151,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2408,7 +2248,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Examples): Add new nn extractors to example configuration files
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="166">
   <si>
     <t xml:space="preserve">CoralSoundExplorer
 Version 1</t>
@@ -638,12 +638,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://sound-scape-explorer.github.io/docs/CSE/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campaign user guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://sound-scape-explorer.github.io/docs/modules/campaign/user-guide/</t>
   </si>
   <si>
     <t xml:space="preserve">setting</t>
@@ -1184,6 +1178,18 @@
   </si>
   <si>
     <t xml:space="preserve">The VGGish neural network.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The melogram (VGGish input)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melspectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The melspectrum (over 1s with same other parameters than melogram)</t>
   </si>
   <si>
     <t xml:space="preserve">The silhouette between subtypes of a given cluster.</t>
@@ -1679,7 +1685,7 @@
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI13"/>
+  <dimension ref="A1:AMI12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -1754,14 +1760,6 @@
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B5"/>
@@ -1769,7 +1767,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="https://sound-scape-explorer.github.io/docs/CSE/"/>
-    <hyperlink ref="B13" r:id="rId2" display="https://sound-scape-explorer.github.io/docs/modules/campaign/user-guide/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1807,24 +1804,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="D1" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="E1" s="42" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B2" s="38" t="n">
         <v>2</v>
@@ -1835,7 +1832,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="37" t="n">
         <v>3</v>
@@ -1889,24 +1886,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="D1" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="E1" s="40" t="s">
         <v>153</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="38" t="n">
         <v>15</v>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3" s="37" t="n">
         <v>15</v>
@@ -1983,31 +1980,41 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="59.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="48"/>
-    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="48"/>
+      <c r="A4" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="48"/>
@@ -2063,26 +2070,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,17 +2148,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2189,17 +2196,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2233,22 +2240,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2286,68 +2293,68 @@
   <sheetData>
     <row r="1" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AMJ1" s="14"/>
     </row>
     <row r="2" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>13</v>
       </c>
       <c r="AMJ2" s="14"/>
     </row>
     <row r="3" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>16</v>
       </c>
       <c r="AMJ3" s="14"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="16" t="n">
         <v>44100</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AMJ4" s="14"/>
     </row>
     <row r="5" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="18" t="n">
         <v>44197</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AMJ5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -3373,49 +3380,49 @@
     </row>
     <row r="7" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>25</v>
       </c>
       <c r="AMJ7" s="14"/>
     </row>
     <row r="8" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="22" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AMJ8" s="14"/>
     </row>
     <row r="9" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="22" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AMJ9" s="14"/>
     </row>
     <row r="10" s="13" customFormat="true" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="22" t="n">
         <v>42000</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AMJ10" s="14"/>
     </row>
@@ -3462,75 +3469,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="I1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="K1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="L1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="M1" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="31" t="n">
         <v>44881.5034722222</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="26" t="n">
         <v>2022</v>
@@ -3545,22 +3552,22 @@
         <v>5</v>
       </c>
       <c r="I2" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L2" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M2" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O2" s="27" t="n">
         <v>465</v>
@@ -3581,16 +3588,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="31" t="n">
         <v>44881.5104166667</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>2022</v>
@@ -3605,22 +3612,22 @@
         <v>5</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L3" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M3" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N3" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O3" s="27" t="n">
         <v>465</v>
@@ -3641,16 +3648,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="31" t="n">
         <v>44881.5173611111</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>2022</v>
@@ -3665,22 +3672,22 @@
         <v>5</v>
       </c>
       <c r="I4" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L4" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M4" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O4" s="27" t="n">
         <v>465</v>
@@ -3701,16 +3708,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="32" t="n">
         <v>44887.5</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>2022</v>
@@ -3725,22 +3732,22 @@
         <v>5</v>
       </c>
       <c r="I5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L5" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N5" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O5" s="27" t="n">
         <v>465</v>
@@ -3761,16 +3768,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="32" t="n">
         <v>44887.5069444444</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>2022</v>
@@ -3785,22 +3792,22 @@
         <v>5</v>
       </c>
       <c r="I6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L6" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O6" s="27" t="n">
         <v>465</v>
@@ -3821,16 +3828,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="32" t="n">
         <v>44887.5138888889</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>2022</v>
@@ -3845,22 +3852,22 @@
         <v>5</v>
       </c>
       <c r="I7" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L7" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M7" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O7" s="27" t="n">
         <v>465</v>
@@ -3881,16 +3888,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="32" t="n">
         <v>44907.5034722222</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>2022</v>
@@ -3905,22 +3912,22 @@
         <v>5</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L8" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M8" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N8" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O8" s="27" t="n">
         <v>465</v>
@@ -3941,16 +3948,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="32" t="n">
         <v>44907.5104166667</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>2022</v>
@@ -3965,22 +3972,22 @@
         <v>5</v>
       </c>
       <c r="I9" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L9" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O9" s="27" t="n">
         <v>465</v>
@@ -4001,16 +4008,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="32" t="n">
         <v>44907.5173611111</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>2022</v>
@@ -4025,22 +4032,22 @@
         <v>5</v>
       </c>
       <c r="I10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L10" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O10" s="27" t="n">
         <v>465</v>
@@ -4061,16 +4068,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="32" t="n">
         <v>44881.5034722222</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" s="26" t="n">
         <v>2022</v>
@@ -4085,22 +4092,22 @@
         <v>2</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N11" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O11" s="27" t="n">
         <v>378</v>
@@ -4121,16 +4128,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="32" t="n">
         <v>44881.5104166667</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" s="26" t="n">
         <v>2022</v>
@@ -4145,22 +4152,22 @@
         <v>2</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M12" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N12" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O12" s="27" t="n">
         <v>378</v>
@@ -4181,16 +4188,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="32" t="n">
         <v>44881.5173611111</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" s="26" t="n">
         <v>2022</v>
@@ -4205,22 +4212,22 @@
         <v>2</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N13" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O13" s="27" t="n">
         <v>378</v>
@@ -4241,16 +4248,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="32" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="26" t="n">
         <v>2022</v>
@@ -4265,22 +4272,22 @@
         <v>2</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L14" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N14" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O14" s="27" t="n">
         <v>378</v>
@@ -4301,16 +4308,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="32" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" s="26" t="n">
         <v>2022</v>
@@ -4325,22 +4332,22 @@
         <v>2</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L15" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M15" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N15" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O15" s="27" t="n">
         <v>378</v>
@@ -4361,16 +4368,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="32" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" s="26" t="n">
         <v>2022</v>
@@ -4385,22 +4392,22 @@
         <v>2</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K16" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L16" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M16" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N16" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O16" s="27" t="n">
         <v>378</v>
@@ -4421,16 +4428,16 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="32" t="n">
         <v>44907.5</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E17" s="26" t="n">
         <v>2022</v>
@@ -4445,22 +4452,22 @@
         <v>2</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L17" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O17" s="27" t="n">
         <v>378</v>
@@ -4481,16 +4488,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" s="32" t="n">
         <v>44907.5069444444</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E18" s="26" t="n">
         <v>2022</v>
@@ -4505,22 +4512,22 @@
         <v>2</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K18" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L18" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M18" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O18" s="27" t="n">
         <v>378</v>
@@ -4541,16 +4548,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="32" t="n">
         <v>44907.5138888889</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" s="26" t="n">
         <v>2022</v>
@@ -4565,22 +4572,22 @@
         <v>2</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K19" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L19" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M19" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N19" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O19" s="27" t="n">
         <v>378</v>
@@ -4601,16 +4608,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="32" t="n">
         <v>44881.5</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E20" s="26" t="n">
         <v>2022</v>
@@ -4625,22 +4632,22 @@
         <v>2</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K20" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M20" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N20" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O20" s="27" t="n">
         <v>509</v>
@@ -4661,16 +4668,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="32" t="n">
         <v>44881.5069444444</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E21" s="26" t="n">
         <v>2022</v>
@@ -4685,22 +4692,22 @@
         <v>2</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K21" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L21" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M21" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N21" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O21" s="27" t="n">
         <v>509</v>
@@ -4721,16 +4728,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" s="32" t="n">
         <v>44881.5138888889</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" s="26" t="n">
         <v>2022</v>
@@ -4745,22 +4752,22 @@
         <v>2</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L22" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M22" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N22" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O22" s="27" t="n">
         <v>509</v>
@@ -4781,16 +4788,16 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="32" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E23" s="26" t="n">
         <v>2022</v>
@@ -4805,22 +4812,22 @@
         <v>2</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L23" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M23" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O23" s="27" t="n">
         <v>509</v>
@@ -4841,16 +4848,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24" s="32" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E24" s="26" t="n">
         <v>2022</v>
@@ -4865,22 +4872,22 @@
         <v>2</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L24" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M24" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N24" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O24" s="27" t="n">
         <v>509</v>
@@ -4901,16 +4908,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" s="32" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25" s="26" t="n">
         <v>2022</v>
@@ -4925,22 +4932,22 @@
         <v>2</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K25" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L25" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M25" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N25" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O25" s="27" t="n">
         <v>509</v>
@@ -4961,16 +4968,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" s="32" t="n">
         <v>44907.5034722222</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26" s="26" t="n">
         <v>2022</v>
@@ -4985,22 +4992,22 @@
         <v>2</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K26" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L26" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M26" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N26" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O26" s="27" t="n">
         <v>509</v>
@@ -5021,16 +5028,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" s="32" t="n">
         <v>44907.5104166667</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E27" s="26" t="n">
         <v>2022</v>
@@ -5045,22 +5052,22 @@
         <v>2</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K27" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L27" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M27" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N27" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O27" s="27" t="n">
         <v>509</v>
@@ -5081,16 +5088,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="32" t="n">
         <v>44907.5173611111</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E28" s="26" t="n">
         <v>2022</v>
@@ -5105,22 +5112,22 @@
         <v>2</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K28" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M28" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N28" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O28" s="27" t="n">
         <v>509</v>
@@ -5141,16 +5148,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" s="32" t="n">
         <v>44243.5013888889</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E29" s="26" t="n">
         <v>2021</v>
@@ -5165,22 +5172,22 @@
         <v>2</v>
       </c>
       <c r="I29" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M29" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N29" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O29" s="27" t="n">
         <v>384</v>
@@ -5201,16 +5208,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" s="32" t="n">
         <v>44243.5090277778</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" s="26" t="n">
         <v>2021</v>
@@ -5225,22 +5232,22 @@
         <v>2</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K30" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L30" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M30" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N30" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O30" s="27" t="n">
         <v>384</v>
@@ -5261,16 +5268,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="32" t="n">
         <v>44243.5166666667</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E31" s="26" t="n">
         <v>2021</v>
@@ -5285,22 +5292,22 @@
         <v>2</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L31" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M31" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N31" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O31" s="27" t="n">
         <v>384</v>
@@ -5321,16 +5328,16 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" s="32" t="n">
         <v>44273.5034722222</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E32" s="26" t="n">
         <v>2021</v>
@@ -5345,22 +5352,22 @@
         <v>2</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K32" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L32" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N32" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O32" s="27" t="n">
         <v>697</v>
@@ -5381,16 +5388,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" s="32" t="n">
         <v>44273.5111111111</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="26" t="n">
         <v>2021</v>
@@ -5405,22 +5412,22 @@
         <v>2</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K33" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L33" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M33" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N33" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O33" s="27" t="n">
         <v>697</v>
@@ -5441,16 +5448,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="32" t="n">
         <v>44273.51875</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E34" s="26" t="n">
         <v>2021</v>
@@ -5465,22 +5472,22 @@
         <v>2</v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K34" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L34" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M34" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N34" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O34" s="27" t="n">
         <v>697</v>
@@ -5501,16 +5508,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35" s="32" t="n">
         <v>44300.5034722222</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E35" s="26" t="n">
         <v>2021</v>
@@ -5525,22 +5532,22 @@
         <v>2</v>
       </c>
       <c r="I35" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J35" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K35" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L35" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M35" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N35" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O35" s="27" t="n">
         <v>1794</v>
@@ -5561,16 +5568,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="32" t="n">
         <v>44300.5111111111</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E36" s="26" t="n">
         <v>2021</v>
@@ -5585,22 +5592,22 @@
         <v>2</v>
       </c>
       <c r="I36" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J36" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K36" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L36" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M36" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N36" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O36" s="27" t="n">
         <v>1794</v>
@@ -5621,16 +5628,16 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" s="32" t="n">
         <v>44300.51875</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E37" s="26" t="n">
         <v>2021</v>
@@ -5645,22 +5652,22 @@
         <v>2</v>
       </c>
       <c r="I37" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K37" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L37" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M37" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N37" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O37" s="27" t="n">
         <v>1794</v>
@@ -5681,16 +5688,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="32" t="n">
         <v>44245.5041666667</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E38" s="26" t="n">
         <v>2021</v>
@@ -5705,22 +5712,22 @@
         <v>5</v>
       </c>
       <c r="I38" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J38" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J38" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K38" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L38" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M38" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N38" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O38" s="27" t="n">
         <v>352</v>
@@ -5741,16 +5748,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="32" t="n">
         <v>44245.5118055556</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E39" s="26" t="n">
         <v>2021</v>
@@ -5765,22 +5772,22 @@
         <v>5</v>
       </c>
       <c r="I39" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J39" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K39" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K39" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L39" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M39" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N39" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O39" s="27" t="n">
         <v>352</v>
@@ -5801,16 +5808,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" s="32" t="n">
         <v>44245.5194444444</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E40" s="26" t="n">
         <v>2021</v>
@@ -5825,22 +5832,22 @@
         <v>5</v>
       </c>
       <c r="I40" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J40" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K40" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J40" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K40" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L40" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M40" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N40" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O40" s="27" t="n">
         <v>352</v>
@@ -5861,16 +5868,16 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" s="32" t="n">
         <v>44271.5027777778</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E41" s="26" t="n">
         <v>2021</v>
@@ -5885,22 +5892,22 @@
         <v>5</v>
       </c>
       <c r="I41" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K41" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J41" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K41" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L41" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M41" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N41" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O41" s="27" t="n">
         <v>497</v>
@@ -5921,16 +5928,16 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="32" t="n">
         <v>44271.5104166667</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E42" s="26" t="n">
         <v>2021</v>
@@ -5945,22 +5952,22 @@
         <v>5</v>
       </c>
       <c r="I42" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K42" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J42" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K42" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L42" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M42" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N42" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O42" s="27" t="n">
         <v>497</v>
@@ -5981,16 +5988,16 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C43" s="32" t="n">
         <v>44271.5180555556</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E43" s="26" t="n">
         <v>2021</v>
@@ -6005,22 +6012,22 @@
         <v>5</v>
       </c>
       <c r="I43" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K43" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J43" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K43" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L43" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M43" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N43" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O43" s="27" t="n">
         <v>497</v>
@@ -6041,16 +6048,16 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C44" s="32" t="n">
         <v>44305.5027777778</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E44" s="26" t="n">
         <v>2021</v>
@@ -6065,22 +6072,22 @@
         <v>5</v>
       </c>
       <c r="I44" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J44" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K44" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J44" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K44" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L44" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M44" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N44" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O44" s="27" t="n">
         <v>1178</v>
@@ -6101,16 +6108,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="32" t="n">
         <v>44305.5104166667</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E45" s="26" t="n">
         <v>2021</v>
@@ -6125,22 +6132,22 @@
         <v>5</v>
       </c>
       <c r="I45" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K45" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J45" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K45" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L45" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M45" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N45" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O45" s="27" t="n">
         <v>1178</v>
@@ -6161,16 +6168,16 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C46" s="32" t="n">
         <v>44305.5180555556</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E46" s="26" t="n">
         <v>2021</v>
@@ -6185,22 +6192,22 @@
         <v>5</v>
       </c>
       <c r="I46" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="J46" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="K46" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J46" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="K46" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="L46" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M46" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N46" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O46" s="27" t="n">
         <v>1178</v>
@@ -6221,16 +6228,16 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C47" s="32" t="n">
         <v>44243.5055555556</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E47" s="26" t="n">
         <v>2021</v>
@@ -6245,22 +6252,22 @@
         <v>2</v>
       </c>
       <c r="I47" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K47" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L47" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M47" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N47" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O47" s="27" t="n">
         <v>387</v>
@@ -6281,16 +6288,16 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C48" s="32" t="n">
         <v>44243.5131944445</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E48" s="26" t="n">
         <v>2021</v>
@@ -6305,22 +6312,22 @@
         <v>2</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K48" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L48" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M48" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N48" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O48" s="27" t="n">
         <v>387</v>
@@ -6341,16 +6348,16 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C49" s="32" t="n">
         <v>44243.5208333333</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E49" s="26" t="n">
         <v>2021</v>
@@ -6365,22 +6372,22 @@
         <v>2</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J49" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K49" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L49" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M49" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N49" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O49" s="27" t="n">
         <v>387</v>
@@ -6401,16 +6408,16 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50" s="32" t="n">
         <v>44273.5</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E50" s="26" t="n">
         <v>2021</v>
@@ -6425,22 +6432,22 @@
         <v>2</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J50" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K50" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L50" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M50" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N50" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O50" s="27" t="n">
         <v>680</v>
@@ -6461,16 +6468,16 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C51" s="32" t="n">
         <v>44273.5076388889</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E51" s="26" t="n">
         <v>2021</v>
@@ -6485,22 +6492,22 @@
         <v>2</v>
       </c>
       <c r="I51" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K51" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L51" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M51" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N51" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O51" s="27" t="n">
         <v>680</v>
@@ -6521,16 +6528,16 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C52" s="32" t="n">
         <v>44273.5152777778</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E52" s="26" t="n">
         <v>2021</v>
@@ -6545,22 +6552,22 @@
         <v>2</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J52" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K52" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L52" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M52" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N52" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O52" s="27" t="n">
         <v>680</v>
@@ -6581,16 +6588,16 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C53" s="32" t="n">
         <v>44299.5069444445</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E53" s="26" t="n">
         <v>2021</v>
@@ -6605,22 +6612,22 @@
         <v>2</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K53" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L53" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M53" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N53" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O53" s="27" t="n">
         <v>1258</v>
@@ -6641,16 +6648,16 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C54" s="32" t="n">
         <v>44299.5145833333</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E54" s="26" t="n">
         <v>2021</v>
@@ -6665,22 +6672,22 @@
         <v>2</v>
       </c>
       <c r="I54" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K54" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L54" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M54" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N54" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O54" s="27" t="n">
         <v>1258</v>
@@ -6701,16 +6708,16 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C55" s="32" t="n">
         <v>44299.5222222222</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E55" s="26" t="n">
         <v>2021</v>
@@ -6725,22 +6732,22 @@
         <v>2</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J55" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K55" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L55" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M55" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N55" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O55" s="27" t="n">
         <v>1258</v>
@@ -6794,18 +6801,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>115</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>70</v>
@@ -6861,15 +6868,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>15</v>
@@ -6920,18 +6927,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>44562.5</v>
@@ -6942,7 +6949,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="31" t="n">
         <v>44881.5</v>
@@ -6953,7 +6960,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="32" t="n">
         <v>44887.5</v>
@@ -6964,7 +6971,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="32" t="n">
         <v>44907.5</v>
@@ -7009,27 +7016,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>44881.5</v>
@@ -7038,18 +7045,18 @@
         <v>44882.5034722222</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" s="31" t="n">
         <v>44887.5</v>
@@ -7058,18 +7065,18 @@
         <v>44888.5034722222</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" s="31" t="n">
         <v>44907.5</v>
@@ -7078,13 +7085,13 @@
         <v>44908.5034722222</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7143,21 +7150,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>138</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="37" t="n">
         <v>0</v>
@@ -7166,7 +7173,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" s="39" t="str">
         <f aca="false">VLOOKUP(A2,ListExtractors!$A$2:$B$1048576,2,0)</f>
@@ -7213,12 +7220,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" s="39" t="str">
         <f aca="false">VLOOKUP(A2,ListDigesters!$A$2:$B$1048576,2,0)</f>
@@ -7227,7 +7234,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" s="39" t="str">
         <f aca="false">VLOOKUP(A3,ListDigesters!$A$2:$B$1048576,2,0)</f>

</xml_diff>